<commit_message>
Created method __init__ whit CNN layers in class EurSatCNN
</commit_message>
<xml_diff>
--- a/dl_eurosat_info.xlsx
+++ b/dl_eurosat_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoOne\OneDrive - BTT GROUP UAB\Documents\AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoOne\OneDrive - BTT GROUP UAB\Documents\AI\4_DL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C980A920-8843-4644-86CA-92226C6CC47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93467DE8-7EDA-4BFA-A3CD-89812F32B3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28622" yWindow="-119" windowWidth="28741" windowHeight="15677" activeTab="2" xr2:uid="{91D2B0CB-E679-46A0-A3B7-B64E998F5A43}"/>
+    <workbookView xWindow="-119" yWindow="-119" windowWidth="28741" windowHeight="15677" activeTab="2" xr2:uid="{91D2B0CB-E679-46A0-A3B7-B64E998F5A43}"/>
   </bookViews>
   <sheets>
     <sheet name="check_data" sheetId="1" r:id="rId1"/>
@@ -421,50 +421,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD53E22-3538-4330-A519-B17291CA8F6D}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
@@ -1070,110 +1070,110 @@
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="13"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="13"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="15"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
created EurSatCNN module architecture
</commit_message>
<xml_diff>
--- a/dl_eurosat_info.xlsx
+++ b/dl_eurosat_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoOne\OneDrive - BTT GROUP UAB\Documents\AI\4_DL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93467DE8-7EDA-4BFA-A3CD-89812F32B3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661FFC0-AF49-429C-AAE2-D7DAF658BEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-119" yWindow="-119" windowWidth="28741" windowHeight="15677" activeTab="2" xr2:uid="{91D2B0CB-E679-46A0-A3B7-B64E998F5A43}"/>
   </bookViews>
@@ -967,7 +967,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>

</xml_diff>